<commit_message>
wip: Import Student By Excel
</commit_message>
<xml_diff>
--- a/public/excel_import_template/students_import.xlsx
+++ b/public/excel_import_template/students_import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t xml:space="preserve">Nama</t>
   </si>
@@ -61,9 +61,6 @@
     <t xml:space="preserve">Alamat Ayah</t>
   </si>
   <si>
-    <t xml:space="preserve">Pekerjaan Ayah</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nomor Telepon Ayah</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t xml:space="preserve">Alamat Ibu</t>
   </si>
   <si>
-    <t xml:space="preserve">Pekerjaan Ibu</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nomor Telepon Ibu</t>
   </si>
   <si>
@@ -85,9 +79,6 @@
     <t xml:space="preserve">Alamat Wali</t>
   </si>
   <si>
-    <t xml:space="preserve">Pekerjaan Wali</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nomor Telepon Wali</t>
   </si>
   <si>
@@ -121,24 +112,15 @@
     <t xml:space="preserve">Jr. Dipenogoro No. 345, Bandung 42213, Banten</t>
   </si>
   <si>
-    <t xml:space="preserve">Penyiar Radio</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ilsa Melani</t>
   </si>
   <si>
-    <t xml:space="preserve">Pegawai Negeri Sipil (PNS)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rachel Wastuti</t>
   </si>
   <si>
     <t xml:space="preserve">Psr. Halim No. 905, Sawahlunto 14347, DIY</t>
   </si>
   <si>
-    <t xml:space="preserve">Paraji</t>
-  </si>
-  <si>
     <t xml:space="preserve">Siska Betania Yuliarti S.Farm</t>
   </si>
   <si>
@@ -151,6 +133,9 @@
     <t xml:space="preserve">Ds. Muwardi No. 392, Padangsidempuan 94704, Sulteng</t>
   </si>
   <si>
+    <t xml:space="preserve">08/03/2003</t>
+  </si>
+  <si>
     <t xml:space="preserve">085812429402</t>
   </si>
   <si>
@@ -166,18 +151,12 @@
     <t xml:space="preserve">Gg. Suryo No. 182, Payakumbuh 97153, Riau</t>
   </si>
   <si>
-    <t xml:space="preserve">Perancang Busana</t>
-  </si>
-  <si>
     <t xml:space="preserve">Queen Suartini</t>
   </si>
   <si>
     <t xml:space="preserve">Kpg. Gading No. 791, Lhokseumawe 74003, Bengkulu</t>
   </si>
   <si>
-    <t xml:space="preserve">Konstruksi</t>
-  </si>
-  <si>
     <t xml:space="preserve">Maras Bahuraksa Iswahyudi</t>
   </si>
   <si>
@@ -187,6 +166,9 @@
     <t xml:space="preserve">Jr. Asia Afrika No. 790, Sungai Penuh 42835, Kalsel</t>
   </si>
   <si>
+    <t xml:space="preserve">04/26/2004</t>
+  </si>
+  <si>
     <t xml:space="preserve">089285782935</t>
   </si>
   <si>
@@ -202,22 +184,13 @@
     <t xml:space="preserve">Ds. Supomo No. 961, Palembang 80017, Bali</t>
   </si>
   <si>
-    <t xml:space="preserve">Transportasi</t>
-  </si>
-  <si>
     <t xml:space="preserve">Shania Widiastuti M.Pd</t>
   </si>
   <si>
-    <t xml:space="preserve">Karyawan Swasta</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yuliana Usyi Halimah</t>
   </si>
   <si>
     <t xml:space="preserve">Ds. Tubagus Ismail No. 951, Magelang 63012, Kalbar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Penata Busana</t>
   </si>
 </sst>
 </file>
@@ -414,16 +387,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V3" activeCellId="0" sqref="V3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S4" activeCellId="0" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="1" style="1" width="30.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="24" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="1" style="1" width="30.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="21" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="10.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,43 +461,34 @@
       <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E2" s="4" t="n">
         <v>37948</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>715311312</v>
@@ -532,69 +497,60 @@
         <v>117047387</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>706946036</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>611875383</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="1" t="n">
-        <v>706946036</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>611875383</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="W2" s="1" t="n">
+      <c r="T2" s="1" t="n">
         <v>987958880</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>37836</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>533685358</v>
@@ -603,58 +559,52 @@
         <v>983472148</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="N3" s="1" t="n">
         <v>806298070</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="S3" s="1" t="n">
+      <c r="O3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q3" s="1" t="n">
         <v>133124861</v>
       </c>
-      <c r="U3" s="0"/>
+      <c r="S3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="4" t="n">
-        <v>38103</v>
+        <v>47</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J4" s="1" t="n">
         <v>130112285</v>
@@ -663,39 +613,30 @@
         <v>396580957</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O4" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="N4" s="1" t="n">
         <v>491574179</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>59</v>
+      <c r="O4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" s="1" t="n">
+        <v>206641846</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="S4" s="1" t="n">
-        <v>206641846</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="W4" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4" s="1" t="n">
         <v>482675675</v>
       </c>
     </row>

</xml_diff>

<commit_message>
wip: Student Tuition Masters (#74)
* chore: sort student by latest

* chore: additional datatable action links

* wip: Import Student By Excel

* wip: Student Tuitions Master

* Merge branch 'dev' into dev-indra-student
</commit_message>
<xml_diff>
--- a/public/excel_import_template/students_import.xlsx
+++ b/public/excel_import_template/students_import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t xml:space="preserve">Nama</t>
   </si>
@@ -61,9 +61,6 @@
     <t xml:space="preserve">Alamat Ayah</t>
   </si>
   <si>
-    <t xml:space="preserve">Pekerjaan Ayah</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nomor Telepon Ayah</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t xml:space="preserve">Alamat Ibu</t>
   </si>
   <si>
-    <t xml:space="preserve">Pekerjaan Ibu</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nomor Telepon Ibu</t>
   </si>
   <si>
@@ -85,9 +79,6 @@
     <t xml:space="preserve">Alamat Wali</t>
   </si>
   <si>
-    <t xml:space="preserve">Pekerjaan Wali</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nomor Telepon Wali</t>
   </si>
   <si>
@@ -121,24 +112,15 @@
     <t xml:space="preserve">Jr. Dipenogoro No. 345, Bandung 42213, Banten</t>
   </si>
   <si>
-    <t xml:space="preserve">Penyiar Radio</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ilsa Melani</t>
   </si>
   <si>
-    <t xml:space="preserve">Pegawai Negeri Sipil (PNS)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rachel Wastuti</t>
   </si>
   <si>
     <t xml:space="preserve">Psr. Halim No. 905, Sawahlunto 14347, DIY</t>
   </si>
   <si>
-    <t xml:space="preserve">Paraji</t>
-  </si>
-  <si>
     <t xml:space="preserve">Siska Betania Yuliarti S.Farm</t>
   </si>
   <si>
@@ -151,6 +133,9 @@
     <t xml:space="preserve">Ds. Muwardi No. 392, Padangsidempuan 94704, Sulteng</t>
   </si>
   <si>
+    <t xml:space="preserve">08/03/2003</t>
+  </si>
+  <si>
     <t xml:space="preserve">085812429402</t>
   </si>
   <si>
@@ -166,18 +151,12 @@
     <t xml:space="preserve">Gg. Suryo No. 182, Payakumbuh 97153, Riau</t>
   </si>
   <si>
-    <t xml:space="preserve">Perancang Busana</t>
-  </si>
-  <si>
     <t xml:space="preserve">Queen Suartini</t>
   </si>
   <si>
     <t xml:space="preserve">Kpg. Gading No. 791, Lhokseumawe 74003, Bengkulu</t>
   </si>
   <si>
-    <t xml:space="preserve">Konstruksi</t>
-  </si>
-  <si>
     <t xml:space="preserve">Maras Bahuraksa Iswahyudi</t>
   </si>
   <si>
@@ -187,6 +166,9 @@
     <t xml:space="preserve">Jr. Asia Afrika No. 790, Sungai Penuh 42835, Kalsel</t>
   </si>
   <si>
+    <t xml:space="preserve">04/26/2004</t>
+  </si>
+  <si>
     <t xml:space="preserve">089285782935</t>
   </si>
   <si>
@@ -202,22 +184,13 @@
     <t xml:space="preserve">Ds. Supomo No. 961, Palembang 80017, Bali</t>
   </si>
   <si>
-    <t xml:space="preserve">Transportasi</t>
-  </si>
-  <si>
     <t xml:space="preserve">Shania Widiastuti M.Pd</t>
   </si>
   <si>
-    <t xml:space="preserve">Karyawan Swasta</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yuliana Usyi Halimah</t>
   </si>
   <si>
     <t xml:space="preserve">Ds. Tubagus Ismail No. 951, Magelang 63012, Kalbar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Penata Busana</t>
   </si>
 </sst>
 </file>
@@ -414,16 +387,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V3" activeCellId="0" sqref="V3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S4" activeCellId="0" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="1" style="1" width="30.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="24" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="1" style="1" width="30.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="21" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="10.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,43 +461,34 @@
       <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E2" s="4" t="n">
         <v>37948</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>715311312</v>
@@ -532,69 +497,60 @@
         <v>117047387</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>706946036</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>611875383</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="1" t="n">
-        <v>706946036</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>611875383</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="W2" s="1" t="n">
+      <c r="T2" s="1" t="n">
         <v>987958880</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>37836</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>533685358</v>
@@ -603,58 +559,52 @@
         <v>983472148</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="N3" s="1" t="n">
         <v>806298070</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="S3" s="1" t="n">
+      <c r="O3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q3" s="1" t="n">
         <v>133124861</v>
       </c>
-      <c r="U3" s="0"/>
+      <c r="S3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="4" t="n">
-        <v>38103</v>
+        <v>47</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J4" s="1" t="n">
         <v>130112285</v>
@@ -663,39 +613,30 @@
         <v>396580957</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O4" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="N4" s="1" t="n">
         <v>491574179</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>59</v>
+      <c r="O4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" s="1" t="n">
+        <v>206641846</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="S4" s="1" t="n">
-        <v>206641846</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="W4" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4" s="1" t="n">
         <v>482675675</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Student Report ヾ(≧ ▽ ≦)ゝ (#115)
* chore: sort student by latest

* chore: additional datatable action links

* wip: Import Student By Excel

* wip: Student Tuitions Master

* Merge branch 'dev' into dev-indra-student

* wip: student Tuition Master

* chore: Minor changes Students CRUD

* wip: Student Tuition Master

* wip: Student Master Tuition

* feat: Student Tuition Master

* chore: minor update Student Tuition Master

* fix: Student Tuitions Master Bugs

* feat: Student Import

* wip: Student Tuition Master Test

* chore: Update Topbar style

* wip: Student Report

* wip: Student Report

* feat: Student Report ヾ(≧ ▽ ≦)ゝ
</commit_message>
<xml_diff>
--- a/public/excel_import_template/students_import.xlsx
+++ b/public/excel_import_template/students_import.xlsx
@@ -389,8 +389,8 @@
   </sheetPr>
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S4" activeCellId="0" sqref="S4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
chore: Add Email parent
</commit_message>
<xml_diff>
--- a/public/excel_import_template/students_import.xlsx
+++ b/public/excel_import_template/students_import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
   <si>
     <t xml:space="preserve">Nama</t>
   </si>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">Alamat Ayah</t>
   </si>
   <si>
+    <t xml:space="preserve">Email Ayah</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nomor Telepon Ayah</t>
   </si>
   <si>
@@ -70,6 +73,9 @@
     <t xml:space="preserve">Alamat Ibu</t>
   </si>
   <si>
+    <t xml:space="preserve">Email Ibu</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nomor Telepon Ibu</t>
   </si>
   <si>
@@ -79,6 +85,9 @@
     <t xml:space="preserve">Alamat Wali</t>
   </si>
   <si>
+    <t xml:space="preserve">Email Wali</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nomor Telepon Wali</t>
   </si>
   <si>
@@ -94,7 +103,7 @@
     <t xml:space="preserve">Ki. Gajah No. 737, Madiun 93295, Sultra</t>
   </si>
   <si>
-    <t xml:space="preserve">Kristen</t>
+    <t xml:space="preserve">katolik</t>
   </si>
   <si>
     <t xml:space="preserve">081295728943</t>
@@ -112,6 +121,9 @@
     <t xml:space="preserve">Jr. Dipenogoro No. 345, Bandung 42213, Banten</t>
   </si>
   <si>
+    <t xml:space="preserve">HarjasaParmanSaptono@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ilsa Melani</t>
   </si>
   <si>
@@ -151,6 +163,9 @@
     <t xml:space="preserve">Gg. Suryo No. 182, Payakumbuh 97153, Riau</t>
   </si>
   <si>
+    <t xml:space="preserve">BakimanGalionoIswahyudi@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Queen Suartini</t>
   </si>
   <si>
@@ -187,10 +202,16 @@
     <t xml:space="preserve">Shania Widiastuti M.Pd</t>
   </si>
   <si>
+    <t xml:space="preserve">ShaniaWidiastuti@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yuliana Usyi Halimah</t>
   </si>
   <si>
     <t xml:space="preserve">Ds. Tubagus Ismail No. 951, Magelang 63012, Kalbar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YulianaUsyiHalimah@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -202,7 +223,7 @@
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -232,6 +253,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -289,7 +316,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -307,6 +334,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -387,17 +418,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="1" style="1" width="30.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="21" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="1" style="1" width="30.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="24" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -461,34 +491,43 @@
       <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E2" s="4" t="n">
         <v>37948</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J2" s="1" t="n">
         <v>715311312</v>
@@ -497,60 +536,65 @@
         <v>117047387</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="1" t="n">
         <v>706946036</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="1" t="n">
+      <c r="P2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="4"/>
+      <c r="S2" s="1" t="n">
         <v>611875383</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" s="1" t="n">
+      <c r="T2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" s="4"/>
+      <c r="W2" s="1" t="n">
         <v>987958880</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>533685358</v>
@@ -559,52 +603,57 @@
         <v>983472148</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="1" t="n">
         <v>806298070</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q3" s="1" t="n">
+      <c r="P3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" s="4"/>
+      <c r="S3" s="1" t="n">
         <v>133124861</v>
       </c>
-      <c r="S3" s="0"/>
+      <c r="U3" s="0"/>
+      <c r="V3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="J4" s="1" t="n">
         <v>130112285</v>
@@ -613,36 +662,47 @@
         <v>396580957</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="N4" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="1" t="n">
         <v>491574179</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" s="1" t="n">
+      <c r="P4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S4" s="1" t="n">
         <v>206641846</v>
       </c>
-      <c r="R4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="T4" s="1" t="n">
+      <c r="T4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="W4" s="1" t="n">
         <v>482675675</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="LukitaJamilSiregar@gmail.com"/>
+    <hyperlink ref="N2" r:id="rId2" display="HarjasaParmanSaptono@gmail.com"/>
+    <hyperlink ref="N3" r:id="rId3" display="BakimanGalionoIswahyudi@gmail.com"/>
+    <hyperlink ref="R4" r:id="rId4" display="ShaniaWidiastuti@gmail.com"/>
+    <hyperlink ref="V4" r:id="rId5" display="YulianaUsyiHalimah@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>